<commit_message>
Update to Domain Class List
</commit_message>
<xml_diff>
--- a/Class Diagram List.docx.xlsx
+++ b/Class Diagram List.docx.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yemm2299\Documents\GitHub\635_Team_Proect_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\635_Team_Proect_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E284E-DA2A-4D4F-B869-2DB289B7DB6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Class Diagram List</t>
   </si>
   <si>
-    <t>Patron</t>
-  </si>
-  <si>
     <t>FrontDesk</t>
   </si>
   <si>
@@ -44,22 +42,31 @@
     <t>Order</t>
   </si>
   <si>
-    <t xml:space="preserve">Payment </t>
-  </si>
-  <si>
-    <t>(Credit, cash, Check)</t>
-  </si>
-  <si>
     <t>OrderDetail</t>
   </si>
   <si>
-    <t>Gold, Silver, None</t>
+    <t>Patron Gold</t>
+  </si>
+  <si>
+    <t>Patron Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patron </t>
+  </si>
+  <si>
+    <t>Payment  Credit</t>
+  </si>
+  <si>
+    <t>Payment Cash</t>
+  </si>
+  <si>
+    <t>Payment Check</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,13 +120,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,72 +406,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>